<commit_message>
Tagebuch + GANTT Chart
</commit_message>
<xml_diff>
--- a/Planung/4APC_GanttChart_gr01.xlsx
+++ b/Planung/4APC_GanttChart_gr01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F0F303-B79C-4796-B554-E823DA7F64B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D00295-366B-41BD-BBFF-4C423457E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="876" windowWidth="17280" windowHeight="10596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="8904" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>START DES PLANS</t>
   </si>
@@ -1228,8 +1228,8 @@
   </sheetPr>
   <dimension ref="B1:DP27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="49" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.44140625" defaultRowHeight="30" customHeight="1"/>
@@ -2071,14 +2071,14 @@
       <c r="F18" s="7">
         <v>16</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>25</v>
+      <c r="G18" s="7">
+        <v>47</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="30" customHeight="1">
@@ -2116,7 +2116,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="7">
         <v>41</v>
@@ -2131,7 +2131,7 @@
         <v>25</v>
       </c>
       <c r="I20" s="8">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="30" customHeight="1">
@@ -2142,11 +2142,10 @@
         <v>39</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F21" s="7">
         <v>6</v>
@@ -2173,7 +2172,7 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F22" s="7">
         <v>6</v>
@@ -2200,7 +2199,7 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F23" s="7">
         <v>6</v>
@@ -2227,7 +2226,7 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F24" s="7">
         <v>6</v>

</xml_diff>

<commit_message>
Ganttchart aktualisierung, Tagebuch Nachtrag
</commit_message>
<xml_diff>
--- a/Planung/4APC_GanttChart_gr01.xlsx
+++ b/Planung/4APC_GanttChart_gr01.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D00295-366B-41BD-BBFF-4C423457E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B024E1B9-04C5-1346-BB50-A976A3835FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="8904" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Projektplaner!$B$1:$DO$24</definedName>
+    <definedName name="Plan">ZeitraumInPlan*(Projektplaner!$E1&gt;0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Projektplaner!$3:$4</definedName>
-    <definedName name="Plan">ZeitraumInPlan*(Projektplaner!$E1&gt;0)</definedName>
     <definedName name="ProzentAbgeschlossen">ProzentAbgeschlossenHinter*ZeitraumInPlan</definedName>
     <definedName name="ProzentAbgeschlossenHinter">(Projektplaner!A$4=MEDIAN(Projektplaner!A$4,Projektplaner!$G1,Projektplaner!$G1+Projektplaner!$H1)*(Projektplaner!$G1&gt;0))*((Projektplaner!A$4&lt;(INT(Projektplaner!$G1+Projektplaner!$H1*Projektplaner!$I1)))+(Projektplaner!A$4=Projektplaner!$G1))*(Projektplaner!$I1&gt;0)</definedName>
     <definedName name="Tatsächlich">(ZeitraumInTatsächlich*(Projektplaner!$G1&gt;0))*ZeitraumInPlan</definedName>
@@ -199,9 +199,6 @@
     <t>Erstellung von Wireframes und Mockups</t>
   </si>
   <si>
-    <t>Erarbeitung der User Interface Desgins</t>
-  </si>
-  <si>
     <t>Erstellung des Datenbank-Desgins</t>
   </si>
   <si>
@@ -311,13 +308,16 @@
   </si>
   <si>
     <t>2.0</t>
+  </si>
+  <si>
+    <t>Erarbeitung der User Interface Designs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -763,20 +763,20 @@
     <cellStyle name="% abgeschlossen" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Aktivität" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Bezeichnung" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Planlegende" xfId="14" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Projektüberschriften" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Prozent abgeschlossen" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschriften für Zeiträume" xfId="3" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Zeitraumwert" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
@@ -947,15 +947,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>60960</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>609600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>281940</xdr:colOff>
+          <xdr:colOff>279400</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>139700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1228,22 +1228,22 @@
   </sheetPr>
   <dimension ref="B1:DP27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.44140625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="61.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
-    <col min="5" max="8" width="15.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" style="4" customWidth="1"/>
-    <col min="10" max="29" width="4.44140625" style="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="61.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
+    <col min="5" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="4" customWidth="1"/>
+    <col min="10" max="29" width="4.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:120" ht="60" customHeight="1" thickBot="1">
+    <row r="1" spans="2:120" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="13" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="2:120" ht="21" customHeight="1" thickTop="1" thickBot="1">
+    <row r="2" spans="2:120" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
@@ -1321,7 +1321,7 @@
       <c r="AQ2" s="31"/>
       <c r="AR2" s="31"/>
     </row>
-    <row r="3" spans="2:120" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1">
+    <row r="3" spans="2:120" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="32" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" spans="2:120" ht="15.75" customHeight="1">
+    <row r="4" spans="2:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="33"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="DP4" s="3"/>
     </row>
-    <row r="5" spans="2:120" ht="30" customHeight="1">
+    <row r="5" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:120" ht="30" customHeight="1">
+    <row r="6" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="27" t="s">
         <v>17</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="7">
         <f>E5+F5</f>
@@ -1763,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:120" ht="30" customHeight="1">
+    <row r="7" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>18</v>
       </c>
@@ -1790,9 +1790,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:120" ht="30" customHeight="1">
+    <row r="8" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>26</v>
@@ -1817,12 +1817,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:120" ht="30" customHeight="1">
+    <row r="9" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -1844,15 +1844,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:120" ht="30" customHeight="1">
+    <row r="10" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
@@ -1871,15 +1871,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:120" ht="30" customHeight="1">
+    <row r="11" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="7">
         <v>24</v>
@@ -1897,15 +1897,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:120" ht="30" customHeight="1">
+    <row r="12" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
@@ -1924,15 +1924,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:120" ht="30" customHeight="1">
+    <row r="13" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="7">
         <v>30</v>
@@ -1950,15 +1950,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:120" ht="30" customHeight="1">
+    <row r="14" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="7">
         <v>71</v>
@@ -1976,15 +1976,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:120" ht="30" customHeight="1">
+    <row r="15" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
@@ -2003,15 +2003,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:120" ht="30" customHeight="1">
+    <row r="16" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="7">
         <v>33</v>
@@ -2029,12 +2029,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="30" customHeight="1">
+    <row r="17" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>19</v>
@@ -2055,12 +2055,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="30" customHeight="1">
+    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>19</v>
@@ -2078,15 +2078,15 @@
         <v>25</v>
       </c>
       <c r="I18" s="8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="30" customHeight="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
@@ -2108,15 +2108,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="30" customHeight="1">
+    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="7">
         <v>41</v>
@@ -2134,12 +2134,12 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="30" customHeight="1">
+    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>19</v>
@@ -2160,12 +2160,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1">
+    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>19</v>
@@ -2187,15 +2187,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="30" customHeight="1">
+    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
@@ -2214,15 +2214,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="30" customHeight="1">
+    <row r="24" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
@@ -2241,18 +2241,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="30" customHeight="1">
+    <row r="25" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
     </row>
-    <row r="26" spans="2:9" ht="30" customHeight="1">
+    <row r="26" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="30" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2345,15 +2345,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>60960</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>0</xdr:row>
                     <xdr:rowOff>609600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>281940</xdr:colOff>
+                    <xdr:colOff>279400</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>139700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
Tagebuch und Ganttchart aktualisiert
</commit_message>
<xml_diff>
--- a/Planung/4APC_GanttChart_gr01.xlsx
+++ b/Planung/4APC_GanttChart_gr01.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B024E1B9-04C5-1346-BB50-A976A3835FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7E937B-BF50-49AF-809D-C8F776A7AA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Projektplaner!$B$1:$DO$24</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Projektplaner!$3:$4</definedName>
     <definedName name="Plan">ZeitraumInPlan*(Projektplaner!$E1&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Projektplaner!$3:$4</definedName>
     <definedName name="ProzentAbgeschlossen">ProzentAbgeschlossenHinter*ZeitraumInPlan</definedName>
     <definedName name="ProzentAbgeschlossenHinter">(Projektplaner!A$4=MEDIAN(Projektplaner!A$4,Projektplaner!$G1,Projektplaner!$G1+Projektplaner!$H1)*(Projektplaner!$G1&gt;0))*((Projektplaner!A$4&lt;(INT(Projektplaner!$G1+Projektplaner!$H1*Projektplaner!$I1)))+(Projektplaner!A$4=Projektplaner!$G1))*(Projektplaner!$I1&gt;0)</definedName>
     <definedName name="Tatsächlich">(ZeitraumInTatsächlich*(Projektplaner!$G1&gt;0))*ZeitraumInPlan</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>START DES PLANS</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Risikomanagement</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Erstellung von Wireframes und Mockups</t>
   </si>
   <si>
@@ -317,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -763,20 +760,20 @@
     <cellStyle name="% abgeschlossen" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Aktivität" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Bezeichnung" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Planlegende" xfId="14" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Projektüberschriften" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Prozent abgeschlossen" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Überschriften für Zeiträume" xfId="3" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Zeitraumwert" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
@@ -947,15 +944,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>63500</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>609600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>279400</xdr:colOff>
+          <xdr:colOff>281940</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1228,22 +1225,22 @@
   </sheetPr>
   <dimension ref="B1:DP27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.44140625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="61.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
-    <col min="5" max="8" width="15.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" style="4" customWidth="1"/>
-    <col min="10" max="29" width="4.5" style="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="61.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="2" customWidth="1"/>
+    <col min="5" max="8" width="15.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="4" customWidth="1"/>
+    <col min="10" max="29" width="4.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:120" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:120" ht="60" customHeight="1" thickBot="1">
       <c r="B1" s="13" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1252,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="2:120" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:120" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
@@ -1321,7 +1318,7 @@
       <c r="AQ2" s="31"/>
       <c r="AR2" s="31"/>
     </row>
-    <row r="3" spans="2:120" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:120" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1">
       <c r="B3" s="32" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1366,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" spans="2:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:120" ht="15.75" customHeight="1">
       <c r="B4" s="33"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1710,7 +1707,7 @@
       </c>
       <c r="DP4" s="3"/>
     </row>
-    <row r="5" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:120" ht="30" customHeight="1">
       <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
@@ -1736,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:120" ht="30" customHeight="1">
       <c r="B6" s="27" t="s">
         <v>17</v>
       </c>
@@ -1744,7 +1741,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="7">
         <f>E5+F5</f>
@@ -1763,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:120" ht="30" customHeight="1">
       <c r="B7" s="27" t="s">
         <v>18</v>
       </c>
@@ -1790,12 +1787,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:120" ht="30" customHeight="1">
       <c r="B8" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>19</v>
@@ -1817,12 +1814,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:120" ht="30" customHeight="1">
       <c r="B9" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -1844,15 +1841,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:120" ht="30" customHeight="1">
       <c r="B10" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
@@ -1871,15 +1868,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:120" ht="30" customHeight="1">
       <c r="B11" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="7">
         <v>24</v>
@@ -1897,15 +1894,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:120" ht="30" customHeight="1">
       <c r="B12" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
@@ -1924,15 +1921,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:120" ht="30" customHeight="1">
       <c r="B13" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7">
         <v>30</v>
@@ -1950,15 +1947,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:120" ht="30" customHeight="1">
       <c r="B14" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="7">
         <v>71</v>
@@ -1966,25 +1963,25 @@
       <c r="F14" s="7">
         <v>8</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>25</v>
+      <c r="G14" s="7">
+        <v>71</v>
+      </c>
+      <c r="H14" s="7">
+        <v>5</v>
       </c>
       <c r="I14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:120" ht="30" customHeight="1">
       <c r="B15" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
@@ -1993,25 +1990,25 @@
       <c r="F15" s="7">
         <v>8</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>25</v>
+      <c r="G15" s="7">
+        <v>79</v>
+      </c>
+      <c r="H15" s="7">
+        <v>6</v>
       </c>
       <c r="I15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:120" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:120" ht="30" customHeight="1">
       <c r="B16" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="7">
         <v>33</v>
@@ -2029,12 +2026,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="30" customHeight="1">
       <c r="B17" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>19</v>
@@ -2048,19 +2045,19 @@
       <c r="G17" s="7">
         <v>41</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>25</v>
+      <c r="H17" s="7">
+        <v>10</v>
       </c>
       <c r="I17" s="8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="30" customHeight="1">
       <c r="B18" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>19</v>
@@ -2074,19 +2071,19 @@
       <c r="G18" s="7">
         <v>47</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>25</v>
+      <c r="H18" s="7">
+        <v>16</v>
       </c>
       <c r="I18" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30" customHeight="1">
       <c r="B19" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
@@ -2098,25 +2095,25 @@
       <c r="F19" s="7">
         <v>6</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>25</v>
+      <c r="G19" s="7">
+        <v>63</v>
+      </c>
+      <c r="H19" s="7">
+        <v>6</v>
       </c>
       <c r="I19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="30" customHeight="1">
       <c r="B20" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="7">
         <v>41</v>
@@ -2127,19 +2124,19 @@
       <c r="G20" s="7">
         <v>41</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>25</v>
+      <c r="H20" s="7">
+        <v>6</v>
       </c>
       <c r="I20" s="8">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="30" customHeight="1">
       <c r="B21" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>19</v>
@@ -2150,22 +2147,22 @@
       <c r="F21" s="7">
         <v>6</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>25</v>
+      <c r="G21" s="7">
+        <v>41</v>
+      </c>
+      <c r="H21" s="7">
+        <v>6</v>
       </c>
       <c r="I21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="30" customHeight="1">
       <c r="B22" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>19</v>
@@ -2177,25 +2174,25 @@
       <c r="F22" s="7">
         <v>6</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>25</v>
+      <c r="G22" s="7">
+        <v>47</v>
+      </c>
+      <c r="H22" s="7">
+        <v>3</v>
       </c>
       <c r="I22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="30" customHeight="1">
       <c r="B23" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
@@ -2204,25 +2201,25 @@
       <c r="F23" s="7">
         <v>6</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>25</v>
+      <c r="G23" s="7">
+        <v>53</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0</v>
       </c>
       <c r="I23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="30" customHeight="1">
       <c r="B24" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
@@ -2231,28 +2228,28 @@
       <c r="F24" s="7">
         <v>6</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>25</v>
+      <c r="G24" s="7">
+        <v>59</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0</v>
       </c>
       <c r="I24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="30" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
     </row>
-    <row r="26" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="30" customHeight="1">
       <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="30" customHeight="1">
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2345,15 +2342,15 @@
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>0</xdr:row>
                     <xdr:rowOff>609600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:colOff>281940</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>139700</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>